<commit_message>
UW TC 1 To 4
</commit_message>
<xml_diff>
--- a/automation/Repository/Underwriting.xlsx
+++ b/automation/Repository/Underwriting.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Remittance_Name</t>
   </si>
@@ -78,13 +78,7 @@
     <t>1232</t>
   </si>
   <si>
-    <t>1233</t>
-  </si>
-  <si>
     <t>1212</t>
-  </si>
-  <si>
-    <t>1213</t>
   </si>
   <si>
     <t>Standard</t>
@@ -421,7 +415,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,48 +466,44 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C3" s="1"/>
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
       <c r="H3" t="s">
         <v>14</v>
       </c>
@@ -521,34 +511,30 @@
         <v>16</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>